<commit_message>
ajout NA sur champ vide
</commit_message>
<xml_diff>
--- a/Excel/templates/HCF-LCF CTRL EFFORT FT TestSuite.xlsx
+++ b/Excel/templates/HCF-LCF CTRL EFFORT FT TestSuite.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">FTLCFHCFEFF!$A$1:$K$59</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
   <si>
     <t>DONNEES EPROUVETTE</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>FICHE TECHNIQUE LCF / HCF CONTROLE EFFORT</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -932,20 +935,190 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -956,176 +1129,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1654,7 +1657,7 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="I22" activeCellId="1" sqref="K22 I22"/>
+      <selection activeCell="K52" activeCellId="20" sqref="I7:I12 B7:B9 B13 B15 B16 B17 F17 F16 F15 B23:B25 B28:B30 D28:D30 I28:J31 I22:I25 K22:K24 J17:J18 K20 J49 J46 I52 K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1682,20 +1685,20 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="91"/>
-      <c r="H5" s="89" t="s">
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="140"/>
+      <c r="H5" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="91"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="140"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
@@ -1713,49 +1716,61 @@
       <c r="A7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
+      <c r="B7" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
       <c r="H7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="104"/>
+      <c r="I7" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="89"/>
+      <c r="K7" s="95"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="B8" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="94"/>
       <c r="H8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="101"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="106"/>
+      <c r="I8" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="96"/>
+      <c r="K8" s="97"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="103"/>
+      <c r="B9" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="94"/>
       <c r="H9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="101"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="106"/>
+      <c r="I9" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="96"/>
+      <c r="K9" s="97"/>
     </row>
     <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -1767,41 +1782,49 @@
       <c r="H10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="98"/>
+      <c r="I10" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="J10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="104"/>
+      <c r="K10" s="95"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="104"/>
+      <c r="I11" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="89"/>
+      <c r="K11" s="95"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
+      <c r="B12" s="137"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="25"/>
       <c r="H12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="101"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="106"/>
+      <c r="I12" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="96"/>
+      <c r="K12" s="97"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="98"/>
+      <c r="B13" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="C13" s="26"/>
       <c r="D13" s="27" t="s">
         <v>74</v>
@@ -1817,7 +1840,7 @@
     </row>
     <row r="14" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
-      <c r="B14" s="112"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -1831,13 +1854,17 @@
       <c r="A15" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="98"/>
+      <c r="B15" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="C15" s="26"/>
       <c r="D15" s="27" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="27"/>
-      <c r="F15" s="104"/>
+      <c r="F15" s="95" t="s">
+        <v>90</v>
+      </c>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
@@ -1848,40 +1875,50 @@
       <c r="A16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="98"/>
+      <c r="B16" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="C16" s="26"/>
       <c r="D16" s="27" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="27"/>
-      <c r="F16" s="111"/>
-      <c r="H16" s="89" t="s">
+      <c r="F16" s="102" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="91"/>
+      <c r="I16" s="137"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="140"/>
       <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="98"/>
+      <c r="B17" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="C17" s="29"/>
       <c r="D17" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="111"/>
+      <c r="F17" s="102" t="s">
+        <v>90</v>
+      </c>
       <c r="H17" s="20" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="107"/>
-      <c r="K17" s="108"/>
+      <c r="J17" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="99"/>
       <c r="N17" s="27"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1890,13 +1927,15 @@
       <c r="C18" s="29"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
-      <c r="F18" s="111"/>
+      <c r="F18" s="102"/>
       <c r="H18" s="20"/>
       <c r="I18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="109"/>
-      <c r="K18" s="110"/>
+      <c r="J18" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="101"/>
     </row>
     <row r="19" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
@@ -1914,27 +1953,29 @@
       <c r="H20" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="123"/>
+      <c r="I20" s="114"/>
       <c r="J20" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="124"/>
+      <c r="K20" s="115" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="90"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="91"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="140"/>
       <c r="H21" s="7"/>
       <c r="I21" s="83"/>
       <c r="J21" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="125"/>
+      <c r="K21" s="116"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
@@ -1945,17 +1986,23 @@
       <c r="H22" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="144"/>
+      <c r="I22" s="135" t="s">
+        <v>90</v>
+      </c>
       <c r="J22" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="143"/>
+      <c r="K22" s="134" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="98"/>
+      <c r="B23" s="89" t="s">
+        <v>90</v>
+      </c>
       <c r="C23" s="29"/>
       <c r="D23" s="44" t="s">
         <v>77</v>
@@ -1966,17 +2013,23 @@
       <c r="H23" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="101"/>
+      <c r="I23" s="92" t="s">
+        <v>90</v>
+      </c>
       <c r="J23" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="126"/>
+      <c r="K23" s="117" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="101"/>
+      <c r="B24" s="92" t="s">
+        <v>90</v>
+      </c>
       <c r="C24" s="29"/>
       <c r="D24" s="44" t="s">
         <v>77</v>
@@ -1987,17 +2040,23 @@
       <c r="H24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="142"/>
+      <c r="I24" s="133" t="s">
+        <v>90</v>
+      </c>
       <c r="J24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="141"/>
+      <c r="K24" s="132" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="92" t="s">
+        <v>90</v>
+      </c>
       <c r="C25" s="29"/>
       <c r="D25" s="44" t="s">
         <v>77</v>
@@ -2008,7 +2067,9 @@
       <c r="H25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="142"/>
+      <c r="I25" s="133" t="s">
+        <v>90</v>
+      </c>
       <c r="J25" s="4" t="s">
         <v>35</v>
       </c>
@@ -2052,48 +2113,72 @@
       <c r="A28" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="123"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="128"/>
-      <c r="E28" s="123"/>
+      <c r="B28" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="114"/>
       <c r="F28" s="48"/>
       <c r="H28" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="132"/>
-      <c r="J28" s="133"/>
+      <c r="I28" s="123" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="124" t="s">
+        <v>90</v>
+      </c>
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="138"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="138"/>
+      <c r="B29" s="129" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="130"/>
+      <c r="D29" s="131" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="129"/>
       <c r="F29" s="48"/>
       <c r="H29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="134"/>
-      <c r="J29" s="135"/>
+      <c r="I29" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="126" t="s">
+        <v>90</v>
+      </c>
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="129"/>
-      <c r="C30" s="130"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="129"/>
+      <c r="B30" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="121"/>
+      <c r="D30" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="120"/>
       <c r="F30" s="48"/>
       <c r="H30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="134"/>
-      <c r="J30" s="135"/>
+      <c r="I30" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="126" t="s">
+        <v>90</v>
+      </c>
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -2106,8 +2191,12 @@
       <c r="H31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="136"/>
-      <c r="J31" s="137"/>
+      <c r="I31" s="127" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="128" t="s">
+        <v>90</v>
+      </c>
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2136,10 +2225,10 @@
       <c r="K33" s="51"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="141" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="95"/>
+      <c r="B34" s="142"/>
       <c r="C34" s="52"/>
       <c r="D34" s="85" t="s">
         <v>70</v>
@@ -2151,7 +2240,7 @@
       <c r="I34" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="117"/>
+      <c r="J34" s="108"/>
       <c r="K34" s="53"/>
     </row>
     <row r="35" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2171,13 +2260,13 @@
       <c r="A36" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="108"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="52"/>
       <c r="D36" s="44" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="35"/>
-      <c r="F36" s="107"/>
+      <c r="F36" s="98"/>
       <c r="G36" s="42"/>
       <c r="H36" s="56"/>
       <c r="I36" s="24" t="s">
@@ -2194,20 +2283,20 @@
       <c r="A37" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="92"/>
       <c r="C37" s="58"/>
       <c r="D37" s="44" t="s">
         <v>86</v>
       </c>
       <c r="E37" s="35"/>
-      <c r="F37" s="107"/>
+      <c r="F37" s="98"/>
       <c r="G37" s="44"/>
       <c r="H37" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I37" s="98"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="104"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="95"/>
       <c r="M37" s="44"/>
       <c r="N37" s="29"/>
       <c r="O37" s="44"/>
@@ -2238,19 +2327,19 @@
       <c r="O39" s="44"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="89" t="s">
+      <c r="A40" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="90"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="90"/>
-      <c r="G40" s="90"/>
-      <c r="H40" s="90"/>
-      <c r="I40" s="90"/>
-      <c r="J40" s="90"/>
-      <c r="K40" s="91"/>
+      <c r="B40" s="137"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="137"/>
+      <c r="E40" s="137"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="137"/>
+      <c r="I40" s="137"/>
+      <c r="J40" s="137"/>
+      <c r="K40" s="140"/>
       <c r="M40" s="44"/>
       <c r="N40" s="44"/>
       <c r="O40" s="44"/>
@@ -2313,27 +2402,27 @@
       <c r="S43" s="44"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="89" t="s">
+      <c r="A44" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="90"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="96" t="s">
+      <c r="B44" s="137"/>
+      <c r="C44" s="137"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="140"/>
+      <c r="J44" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="K44" s="97"/>
+      <c r="K44" s="144"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="118"/>
+      <c r="B45" s="109"/>
       <c r="C45" s="44"/>
       <c r="E45" s="42" t="s">
         <v>68</v>
@@ -2343,7 +2432,7 @@
         <v>51</v>
       </c>
       <c r="H45" s="44"/>
-      <c r="I45" s="121"/>
+      <c r="I45" s="112"/>
       <c r="J45" s="72" t="s">
         <v>47</v>
       </c>
@@ -2361,14 +2450,16 @@
       </c>
       <c r="H46" s="44"/>
       <c r="I46" s="44"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="116"/>
+      <c r="J46" s="106" t="s">
+        <v>90</v>
+      </c>
+      <c r="K46" s="107"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="107"/>
+      <c r="B47" s="98"/>
       <c r="C47" s="44"/>
       <c r="D47" s="44"/>
       <c r="E47" s="44"/>
@@ -2377,7 +2468,7 @@
         <v>52</v>
       </c>
       <c r="H47" s="44"/>
-      <c r="I47" s="108"/>
+      <c r="I47" s="99"/>
       <c r="J47" s="71" t="s">
         <v>48</v>
       </c>
@@ -2401,17 +2492,19 @@
         <v>87</v>
       </c>
       <c r="B49" s="77"/>
-      <c r="C49" s="122"/>
-      <c r="D49" s="122"/>
-      <c r="E49" s="122"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="113"/>
+      <c r="E49" s="113"/>
       <c r="F49" s="78" t="s">
         <v>55</v>
       </c>
       <c r="G49" s="77"/>
-      <c r="H49" s="122"/>
+      <c r="H49" s="113"/>
       <c r="I49" s="44"/>
-      <c r="J49" s="113"/>
-      <c r="K49" s="114"/>
+      <c r="J49" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="K49" s="105"/>
     </row>
     <row r="50" spans="1:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
@@ -2423,8 +2516,8 @@
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
-      <c r="J50" s="92"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="138"/>
+      <c r="K50" s="139"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2440,11 +2533,15 @@
       <c r="H52" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I52" s="119"/>
+      <c r="I52" s="110" t="s">
+        <v>90</v>
+      </c>
       <c r="J52" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="K52" s="120"/>
+      <c r="K52" s="111" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
@@ -2541,6 +2638,8 @@
   </sheetData>
   <sheetProtection password="CDCA"/>
   <mergeCells count="10">
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="H5:K5"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="H16:K16"/>
@@ -2549,8 +2648,6 @@
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A44:I44"/>
     <mergeCell ref="J44:K44"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
update temperature STL et nombre chiffre virgule
</commit_message>
<xml_diff>
--- a/Excel/templates/HCF-LCF CTRL EFFORT FT TestSuite.xlsx
+++ b/Excel/templates/HCF-LCF CTRL EFFORT FT TestSuite.xlsx
@@ -342,8 +342,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="###\ ###\ ###\ ###\ ###\ "/>
-    <numFmt numFmtId="168" formatCode="0.0##"/>
+    <numFmt numFmtId="166" formatCode="###\ ###\ ###\ ###\ ###\ "/>
+    <numFmt numFmtId="167" formatCode="0.0##"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1020,10 +1020,6 @@
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
@@ -1092,11 +1088,19 @@
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,11 +1127,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1686,20 +1686,20 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="136"/>
-      <c r="H5" s="134" t="s">
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="137"/>
+      <c r="H5" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="135"/>
-      <c r="J5" s="135"/>
-      <c r="K5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="137"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
@@ -1802,13 +1802,13 @@
       <c r="K11" s="95"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="135"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="135"/>
-      <c r="E12" s="135"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
       <c r="F12" s="25"/>
       <c r="H12" s="20" t="s">
         <v>8</v>
@@ -1887,12 +1887,12 @@
       <c r="F16" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="134" t="s">
+      <c r="H16" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="135"/>
-      <c r="J16" s="135"/>
-      <c r="K16" s="136"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
+      <c r="K16" s="137"/>
       <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1963,20 +1963,20 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134" t="s">
+      <c r="A21" s="135" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="135"/>
-      <c r="C21" s="135"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="136"/>
+      <c r="B21" s="136"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="137"/>
       <c r="H21" s="7"/>
       <c r="I21" s="83"/>
       <c r="J21" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="114"/>
+      <c r="K21" s="144"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
@@ -1987,13 +1987,13 @@
       <c r="H22" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="144" t="s">
+      <c r="I22" s="134" t="s">
         <v>90</v>
       </c>
       <c r="J22" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="143" t="s">
+      <c r="K22" s="133" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
       <c r="J23" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="115" t="s">
+      <c r="K23" s="114" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2041,13 +2041,13 @@
       <c r="H24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="131" t="s">
+      <c r="I24" s="130" t="s">
         <v>90</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="130" t="s">
+      <c r="K24" s="129" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
       <c r="H25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="131" t="s">
+      <c r="I25" s="130" t="s">
         <v>90</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -2117,8 +2117,8 @@
       <c r="B28" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117" t="s">
+      <c r="C28" s="115"/>
+      <c r="D28" s="116" t="s">
         <v>90</v>
       </c>
       <c r="E28" s="112"/>
@@ -2126,10 +2126,10 @@
       <c r="H28" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="121" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="122" t="s">
+      <c r="I28" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="121" t="s">
         <v>90</v>
       </c>
       <c r="K28" s="10"/>
@@ -2138,22 +2138,22 @@
       <c r="A29" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="127" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="129" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="127"/>
+      <c r="B29" s="126" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="127"/>
+      <c r="D29" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="126"/>
       <c r="F29" s="48"/>
       <c r="H29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="124" t="s">
+      <c r="I29" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="123" t="s">
         <v>90</v>
       </c>
       <c r="K29" s="10"/>
@@ -2162,22 +2162,22 @@
       <c r="A30" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="118" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="119"/>
-      <c r="D30" s="120" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="118"/>
+      <c r="B30" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="118"/>
+      <c r="D30" s="119" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="117"/>
       <c r="F30" s="48"/>
       <c r="H30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="124" t="s">
+      <c r="I30" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="123" t="s">
         <v>90</v>
       </c>
       <c r="K30" s="10"/>
@@ -2192,10 +2192,10 @@
       <c r="H31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="125" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="126" t="s">
+      <c r="I31" s="124" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="125" t="s">
         <v>90</v>
       </c>
       <c r="K31" s="10"/>
@@ -2226,10 +2226,10 @@
       <c r="K33" s="51"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="139" t="s">
+      <c r="A34" s="140" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="140"/>
+      <c r="B34" s="141"/>
       <c r="C34" s="52"/>
       <c r="D34" s="85" t="s">
         <v>70</v>
@@ -2328,19 +2328,19 @@
       <c r="O39" s="44"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134" t="s">
+      <c r="A40" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="135"/>
-      <c r="C40" s="135"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135"/>
-      <c r="J40" s="135"/>
-      <c r="K40" s="136"/>
+      <c r="B40" s="136"/>
+      <c r="C40" s="136"/>
+      <c r="D40" s="136"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="136"/>
+      <c r="G40" s="136"/>
+      <c r="H40" s="136"/>
+      <c r="I40" s="136"/>
+      <c r="J40" s="136"/>
+      <c r="K40" s="137"/>
       <c r="M40" s="44"/>
       <c r="N40" s="44"/>
       <c r="O40" s="44"/>
@@ -2403,21 +2403,21 @@
       <c r="S43" s="44"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="134" t="s">
+      <c r="A44" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="135"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="135"/>
-      <c r="H44" s="135"/>
-      <c r="I44" s="136"/>
-      <c r="J44" s="141" t="s">
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="136"/>
+      <c r="H44" s="136"/>
+      <c r="I44" s="137"/>
+      <c r="J44" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="K44" s="142"/>
+      <c r="K44" s="143"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="H46" s="44"/>
       <c r="I46" s="44"/>
-      <c r="J46" s="133" t="s">
+      <c r="J46" s="132" t="s">
         <v>90</v>
       </c>
       <c r="K46" s="105"/>
@@ -2502,7 +2502,7 @@
       <c r="G49" s="77"/>
       <c r="H49" s="111"/>
       <c r="I49" s="44"/>
-      <c r="J49" s="132" t="s">
+      <c r="J49" s="131" t="s">
         <v>90</v>
       </c>
       <c r="K49" s="104"/>
@@ -2517,8 +2517,8 @@
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
-      <c r="J50" s="137"/>
-      <c r="K50" s="138"/>
+      <c r="J50" s="138"/>
+      <c r="K50" s="139"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>